<commit_message>
Worked on GGD and checked attendance
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sepi\OneDrive\School\Year 2\DSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sepi\Documents\Important Portable Stuff V1\Year 2\Sexy-Egels\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -650,7 +650,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 6:Week 27'!B8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -697,7 +697,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 6:Week 27'!C8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5">
         <f>B4/(B1/100)</f>
@@ -727,7 +727,7 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 6:Week 27'!D8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5">
         <f>B5/(B1/100)</f>
@@ -757,7 +757,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 6:Week 27'!E8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="5">
         <f>B6/(B1/100)</f>
@@ -787,7 +787,7 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Week 6:Week 27'!F8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5">
         <f>B7/(B1/100)</f>
@@ -817,7 +817,7 @@
       </c>
       <c r="B8" s="5">
         <f>SUM('Week 6:Week 27'!G8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5">
         <f>B8/(B1/100)</f>
@@ -847,7 +847,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5">
         <f>B9/(B1/100)</f>
@@ -3182,7 +3182,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3269,13 +3269,27 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -3326,31 +3340,31 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2+B3+B4+B5+B6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>

</xml_diff>

<commit_message>
GGD edits and Attendance
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 6:Week 27'!B8)</f>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -697,11 +697,11 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 6:Week 27'!C8)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5">
         <f>B4/(B1/100)</f>
-        <v>100</v>
+        <v>52.631578947368418</v>
       </c>
       <c r="D4" s="5">
         <f>SUM('Week 6:Week 27'!C11)</f>
@@ -727,11 +727,11 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 6:Week 27'!D8)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5">
         <f>B5/(B1/100)</f>
-        <v>100</v>
+        <v>52.631578947368418</v>
       </c>
       <c r="D5" s="5">
         <f>SUM('Week 6:Week 27'!D11)</f>
@@ -757,11 +757,11 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 6:Week 27'!E8)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5">
         <f>B6/(B1/100)</f>
-        <v>100</v>
+        <v>52.631578947368418</v>
       </c>
       <c r="D6" s="5">
         <f>SUM('Week 6:Week 27'!E11)</f>
@@ -787,11 +787,11 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Week 6:Week 27'!F8)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5">
         <f>B7/(B1/100)</f>
-        <v>100</v>
+        <v>52.631578947368418</v>
       </c>
       <c r="D7" s="5">
         <f>SUM('Week 6:Week 27'!F11)</f>
@@ -817,11 +817,11 @@
       </c>
       <c r="B8" s="5">
         <f>SUM('Week 6:Week 27'!G8)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5">
         <f>B8/(B1/100)</f>
-        <v>100</v>
+        <v>52.631578947368418</v>
       </c>
       <c r="D8" s="5">
         <f>SUM('Week 6:Week 27'!G11)</f>
@@ -847,11 +847,11 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5">
         <f>B9/(B1/100)</f>
-        <v>100</v>
+        <v>52.631578947368418</v>
       </c>
       <c r="D9" s="5">
         <f>SUM('Week 6:Week 27'!H11)</f>
@@ -3181,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3297,13 +3297,27 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -3311,7 +3325,9 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5">
+        <v>9</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -3340,31 +3356,31 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2+B3+B4+B5+B6)</f>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>

</xml_diff>

<commit_message>
Added Presentation Project Folder
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="25">
   <si>
     <t xml:space="preserve">David </t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Maaike had 2 uurtjes Rijles.</t>
+  </si>
+  <si>
+    <t>Rilana is naar de tandarts</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 6:Week 27'!B8)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -700,7 +703,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 6:Week 27'!C8, F4)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5">
         <f>B4/(B1/100)</f>
@@ -730,7 +733,7 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 6:Week 27'!D8,F5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5">
         <f>B5/(B1/100)</f>
@@ -760,7 +763,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 6:Week 27'!E8,F6)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5">
         <f>B6/(B1/100)</f>
@@ -790,7 +793,7 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Week 6:Week 27'!F8,F7)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5">
         <f>B7/(B1/100)</f>
@@ -810,7 +813,7 @@
       </c>
       <c r="G7" s="14">
         <f>F7/(B1/100)</f>
-        <v>11.111111111111111</v>
+        <v>5.5555555555555554</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -820,7 +823,7 @@
       </c>
       <c r="B8" s="5">
         <f>SUM('Week 6:Week 27'!G8,F8)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5">
         <f>B8/(B1/100)</f>
@@ -836,11 +839,11 @@
       </c>
       <c r="F8" s="14">
         <f>SUM('Week 6:Week 27'!G12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" s="14">
         <f>F8/(B1/100)</f>
-        <v>0</v>
+        <v>11.111111111111111</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -850,7 +853,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8,F9)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5">
         <f>B9/(B1/100)</f>
@@ -3184,7 +3187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -4402,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4462,27 +4465,58 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4</v>
+      </c>
       <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -4490,13 +4524,27 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -4504,13 +4552,27 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="K6" s="1"/>
     </row>
@@ -4533,31 +4595,31 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2+B3+B4+B5+B6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>
@@ -4605,6 +4667,9 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
+      <c r="G12" s="5">
+        <v>4</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>

</xml_diff>

<commit_message>
XML Item database working
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="29">
   <si>
     <t xml:space="preserve">David </t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Vakantie</t>
+  </si>
+  <si>
+    <t>Janneke had een doktors afspraak.</t>
   </si>
 </sst>
 </file>
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E4:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +676,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 6:Week 27'!B8)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -720,7 +723,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 6:Week 27'!C8, F4)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C4" s="19">
         <f>B4/(B1/100)</f>
@@ -750,7 +753,7 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 6:Week 27'!D8,F5)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C5" s="19">
         <f>B5/(B1/100)</f>
@@ -780,7 +783,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 6:Week 27'!E8,F6)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C6" s="19">
         <f>B6/(B1/100)</f>
@@ -796,11 +799,11 @@
       </c>
       <c r="F6" s="14">
         <f>SUM('Week 6:Week 27'!E12)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G6" s="18">
         <f>F6/(B1/100)</f>
-        <v>7.4074074074074066</v>
+        <v>11.111111111111111</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -810,7 +813,7 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Week 6:Week 27'!F8,F7)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C7" s="19">
         <f>B7/(B1/100)</f>
@@ -830,7 +833,7 @@
       </c>
       <c r="G7" s="18">
         <f>F7/(B1/100)</f>
-        <v>3.7037037037037033</v>
+        <v>2.7777777777777777</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -840,7 +843,7 @@
       </c>
       <c r="B8" s="5">
         <f>SUM('Week 6:Week 27'!G8,F8)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C8" s="19">
         <f>B8/(B1/100)</f>
@@ -860,7 +863,7 @@
       </c>
       <c r="G8" s="18">
         <f>F8/(B1/100)</f>
-        <v>22.222222222222221</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -870,7 +873,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8,F9)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C9" s="19">
         <f>B9/(B1/100)</f>
@@ -5253,8 +5256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5299,7 +5302,9 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -5313,27 +5318,58 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4</v>
+      </c>
       <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -5341,13 +5377,27 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -5355,13 +5405,27 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="K6" s="1"/>
     </row>
@@ -5384,31 +5448,31 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2+B3+B4+B5+B6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>
@@ -5456,6 +5520,9 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
+      <c r="E12">
+        <v>4</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>

</xml_diff>

<commit_message>
Attendance and slab UI work
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="30">
   <si>
     <t xml:space="preserve">David </t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Janneke had een doktors afspraak.</t>
+  </si>
+  <si>
+    <t>Walter is Ziek</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyFill="1"/>
@@ -337,6 +340,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -659,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -676,7 +682,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 6:Week 27'!B8)</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -723,7 +729,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 6:Week 27'!C8, F4)</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C4" s="19">
         <f>B4/(B1/100)</f>
@@ -753,7 +759,7 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 6:Week 27'!D8,F5)</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C5" s="19">
         <f>B5/(B1/100)</f>
@@ -783,7 +789,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 6:Week 27'!E8,F6)</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C6" s="19">
         <f>B6/(B1/100)</f>
@@ -803,7 +809,7 @@
       </c>
       <c r="G6" s="18">
         <f>F6/(B1/100)</f>
-        <v>11.111111111111111</v>
+        <v>8.8888888888888893</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -813,7 +819,7 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Week 6:Week 27'!F8,F7)</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C7" s="19">
         <f>B7/(B1/100)</f>
@@ -833,7 +839,7 @@
       </c>
       <c r="G7" s="18">
         <f>F7/(B1/100)</f>
-        <v>2.7777777777777777</v>
+        <v>2.2222222222222223</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -843,7 +849,7 @@
       </c>
       <c r="B8" s="5">
         <f>SUM('Week 6:Week 27'!G8,F8)</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C8" s="19">
         <f>B8/(B1/100)</f>
@@ -863,7 +869,7 @@
       </c>
       <c r="G8" s="18">
         <f>F8/(B1/100)</f>
-        <v>16.666666666666668</v>
+        <v>13.333333333333332</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -873,7 +879,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8,F9)</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C9" s="19">
         <f>B9/(B1/100)</f>
@@ -889,11 +895,11 @@
       </c>
       <c r="F9" s="14">
         <f>SUM('Week 6:Week 27'!H12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9" s="18">
         <f>F9/(B1/100)</f>
-        <v>0</v>
+        <v>4.4444444444444446</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -4726,7 +4732,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5256,8 +5262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5520,7 +5526,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>4</v>
       </c>
       <c r="I12" s="1"/>
@@ -5551,7 +5557,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5610,27 +5616,58 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
       <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -5638,13 +5675,27 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -5652,13 +5703,27 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="K6" s="1"/>
     </row>
@@ -5681,31 +5746,31 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2+B3+B4+B5+B6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>
@@ -5753,6 +5818,9 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
+      <c r="H12" s="20">
+        <v>4</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -5780,7 +5848,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
redid the HUD script quickly.
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="32">
   <si>
     <t xml:space="preserve">David </t>
   </si>
@@ -135,7 +135,13 @@
     <t>Janneke had een doktors afspraak.</t>
   </si>
   <si>
-    <t>Walter is Ziek</t>
+    <t>Hele crew behalve Walter ziek</t>
+  </si>
+  <si>
+    <t>Walter is ziek</t>
+  </si>
+  <si>
+    <t>Gerwin ziek</t>
   </si>
 </sst>
 </file>
@@ -682,7 +688,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 6:Week 27'!B8)</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -729,7 +735,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 6:Week 27'!C8, F4)</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C4" s="19">
         <f>B4/(B1/100)</f>
@@ -745,11 +751,11 @@
       </c>
       <c r="F4" s="14">
         <f>SUM('Week 6:Week 27'!C12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" s="18">
         <f>F4/(B1/100)</f>
-        <v>0</v>
+        <v>3.7037037037037033</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -759,7 +765,7 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 6:Week 27'!D8,F5)</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C5" s="19">
         <f>B5/(B1/100)</f>
@@ -775,11 +781,11 @@
       </c>
       <c r="F5" s="14">
         <f>SUM('Week 6:Week 27'!D12)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G5" s="18">
         <f>F5/(B1/100)</f>
-        <v>0</v>
+        <v>11.111111111111111</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -789,7 +795,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 6:Week 27'!E8,F6)</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C6" s="19">
         <f>B6/(B1/100)</f>
@@ -805,11 +811,11 @@
       </c>
       <c r="F6" s="14">
         <f>SUM('Week 6:Week 27'!E12)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G6" s="18">
         <f>F6/(B1/100)</f>
-        <v>8.8888888888888893</v>
+        <v>11.111111111111111</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -819,7 +825,7 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Week 6:Week 27'!F8,F7)</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C7" s="19">
         <f>B7/(B1/100)</f>
@@ -839,7 +845,7 @@
       </c>
       <c r="G7" s="18">
         <f>F7/(B1/100)</f>
-        <v>2.2222222222222223</v>
+        <v>1.8518518518518516</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -849,7 +855,7 @@
       </c>
       <c r="B8" s="5">
         <f>SUM('Week 6:Week 27'!G8,F8)</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C8" s="19">
         <f>B8/(B1/100)</f>
@@ -865,11 +871,11 @@
       </c>
       <c r="F8" s="14">
         <f>SUM('Week 6:Week 27'!G12)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G8" s="18">
         <f>F8/(B1/100)</f>
-        <v>13.333333333333332</v>
+        <v>14.814814814814813</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -879,7 +885,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8,F9)</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C9" s="19">
         <f>B9/(B1/100)</f>
@@ -899,7 +905,7 @@
       </c>
       <c r="G9" s="18">
         <f>F9/(B1/100)</f>
-        <v>4.4444444444444446</v>
+        <v>3.7037037037037033</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -5262,7 +5268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -5557,7 +5563,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5639,7 +5645,7 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -5679,24 +5685,27 @@
         <v>4</v>
       </c>
       <c r="C5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5">
         <v>4</v>
       </c>
       <c r="G5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" s="5">
         <v>4</v>
       </c>
       <c r="I5" s="1"/>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -5710,7 +5719,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
         <v>8</v>
@@ -5725,6 +5734,9 @@
         <v>8</v>
       </c>
       <c r="I6" s="1"/>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -5750,23 +5762,23 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
+        <v>14</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D8" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
@@ -5818,6 +5830,19 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
+      <c r="C12" s="20">
+        <v>4</v>
+      </c>
+      <c r="D12" s="20">
+        <v>12</v>
+      </c>
+      <c r="E12" s="20">
+        <v>4</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20">
+        <v>4</v>
+      </c>
       <c r="H12" s="20">
         <v>4</v>
       </c>
@@ -5847,8 +5872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5907,13 +5932,27 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="K3" s="1"/>
     </row>
@@ -5921,13 +5960,27 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -5935,13 +5988,27 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -5949,13 +6016,27 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="K6" s="1"/>
     </row>
@@ -5978,31 +6059,31 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2+B3+B4+B5+B6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>

</xml_diff>

<commit_message>
Began work on inventory 2.0 and wrote down attendance
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="34">
   <si>
     <t xml:space="preserve">David </t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Gerwin ziek</t>
+  </si>
+  <si>
+    <t>David Familie bezoek, Gerwin ziek</t>
+  </si>
+  <si>
+    <t>Janneke is ziek</t>
   </si>
 </sst>
 </file>
@@ -688,7 +694,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 6:Week 27'!B8)</f>
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -735,7 +741,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 6:Week 27'!C8, F4)</f>
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C4" s="19">
         <f>B4/(B1/100)</f>
@@ -751,11 +757,11 @@
       </c>
       <c r="F4" s="14">
         <f>SUM('Week 6:Week 27'!C12)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G4" s="18">
         <f>F4/(B1/100)</f>
-        <v>3.7037037037037033</v>
+        <v>9.8360655737704921</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -765,7 +771,7 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 6:Week 27'!D8,F5)</f>
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C5" s="19">
         <f>B5/(B1/100)</f>
@@ -781,11 +787,11 @@
       </c>
       <c r="F5" s="14">
         <f>SUM('Week 6:Week 27'!D12)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G5" s="18">
         <f>F5/(B1/100)</f>
-        <v>11.111111111111111</v>
+        <v>16.393442622950818</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -795,7 +801,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 6:Week 27'!E8,F6)</f>
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C6" s="19">
         <f>B6/(B1/100)</f>
@@ -811,11 +817,11 @@
       </c>
       <c r="F6" s="14">
         <f>SUM('Week 6:Week 27'!E12)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G6" s="18">
         <f>F6/(B1/100)</f>
-        <v>11.111111111111111</v>
+        <v>11.475409836065573</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -825,11 +831,11 @@
       </c>
       <c r="B7" s="5">
         <f>SUM('Week 6:Week 27'!F8,F7)</f>
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C7" s="19">
         <f>B7/(B1/100)</f>
-        <v>100</v>
+        <v>70.491803278688522</v>
       </c>
       <c r="D7" s="5">
         <f>SUM('Week 6:Week 27'!F11)</f>
@@ -845,7 +851,7 @@
       </c>
       <c r="G7" s="18">
         <f>F7/(B1/100)</f>
-        <v>1.8518518518518516</v>
+        <v>1.639344262295082</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -855,7 +861,7 @@
       </c>
       <c r="B8" s="5">
         <f>SUM('Week 6:Week 27'!G8,F8)</f>
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C8" s="19">
         <f>B8/(B1/100)</f>
@@ -875,7 +881,7 @@
       </c>
       <c r="G8" s="18">
         <f>F8/(B1/100)</f>
-        <v>14.814814814814813</v>
+        <v>13.114754098360656</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -885,7 +891,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8,F9)</f>
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C9" s="19">
         <f>B9/(B1/100)</f>
@@ -905,7 +911,7 @@
       </c>
       <c r="G9" s="18">
         <f>F9/(B1/100)</f>
-        <v>3.7037037037037033</v>
+        <v>3.278688524590164</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -5269,7 +5275,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5563,7 +5569,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5635,7 +5641,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" s="5">
         <v>4</v>
@@ -5666,7 +5672,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="5">
         <v>2</v>
@@ -5694,7 +5700,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -5725,7 +5731,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G6" s="5">
         <v>8</v>
@@ -5774,7 +5780,7 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
@@ -5872,8 +5878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5945,7 +5951,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" s="5">
         <v>4</v>
@@ -5973,7 +5979,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="5">
         <v>2</v>
@@ -6001,7 +6007,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G5" s="5">
         <v>4</v>
@@ -6020,16 +6026,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
         <v>8</v>
       </c>
       <c r="F6" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G6" s="5">
         <v>8</v>
@@ -6038,6 +6044,9 @@
         <v>8</v>
       </c>
       <c r="I6" s="1"/>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -6063,19 +6072,19 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D8" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
@@ -6131,6 +6140,12 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
+      <c r="C12" s="5">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>8</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -6157,8 +6172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6231,27 +6246,56 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
       <c r="I4" s="1"/>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -6259,13 +6303,27 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="K6" s="1"/>
     </row>
@@ -6288,31 +6346,31 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2+B3+B4+B5+B6)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:H8" si="0">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>
@@ -6360,6 +6418,9 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>

</xml_diff>

<commit_message>
Inventory functionality at 70%
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="36">
   <si>
     <t xml:space="preserve">David </t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Janneke is ziek</t>
+  </si>
+  <si>
+    <t>Gerwin was ziek</t>
+  </si>
+  <si>
+    <t>Janneke was Ziek, Walter is te laat.</t>
   </si>
 </sst>
 </file>
@@ -677,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,11 +793,11 @@
       </c>
       <c r="F5" s="14">
         <f>SUM('Week 6:Week 27'!D12)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G5" s="18">
         <f>F5/(B1/100)</f>
-        <v>14.285714285714286</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -817,11 +823,11 @@
       </c>
       <c r="F6" s="14">
         <f>SUM('Week 6:Week 27'!E12)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G6" s="18">
         <f>F6/(B1/100)</f>
-        <v>10</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -891,19 +897,19 @@
       </c>
       <c r="B9" s="5">
         <f>SUM('Week 6:Week 27'!H8,F9)</f>
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C9" s="19">
         <f>B9/(B1/100)</f>
-        <v>100</v>
+        <v>97.142857142857153</v>
       </c>
       <c r="D9" s="5">
         <f>SUM('Week 6:Week 27'!H11)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9" s="19">
         <f>D9/(B1/100)</f>
-        <v>0</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="F9" s="14">
         <f>SUM('Week 6:Week 27'!H12)</f>
@@ -935,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <v>4</v>
@@ -1017,6 +1023,9 @@
         <v>4</v>
       </c>
       <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1061,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5">
         <v>4</v>
@@ -1070,9 +1079,12 @@
         <v>4</v>
       </c>
       <c r="H5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1"/>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1130,23 +1142,23 @@
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E8" s="5">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="F8" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="G8" s="5">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>
@@ -1185,6 +1197,9 @@
         <v>20</v>
       </c>
       <c r="B11" s="7"/>
+      <c r="H11">
+        <v>4</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -1194,6 +1209,12 @@
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>

</xml_diff>

<commit_message>
Interaction and slab hand following
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2.xlsx
+++ b/Documents/Aanwezigheid Game labs 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" firstSheet="6" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8412" tabRatio="601" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Percentages" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="41">
   <si>
     <t xml:space="preserve">David </t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Janneke doktor, Rilana ziek;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Arne</t>
   </si>
 </sst>
 </file>
@@ -687,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,7 +709,7 @@
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -715,7 +724,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -725,7 +734,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="17" t="s">
         <v>19</v>
@@ -747,7 +756,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -777,7 +786,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -807,7 +816,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -837,7 +846,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -867,7 +876,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -897,7 +906,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -927,15 +936,80 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="5">
+        <f>SUM('Week 6:Week 27'!I8,F10)</f>
+        <v>186</v>
+      </c>
+      <c r="C10" s="19">
+        <f>B10/(B1/100)</f>
+        <v>100</v>
+      </c>
+      <c r="D10" s="5">
+        <f>SUM('Week 6:Week 27'!H12)</f>
+        <v>10</v>
+      </c>
+      <c r="E10" s="19">
+        <f>D10/(B1/100)</f>
+        <v>5.376344086021505</v>
+      </c>
+      <c r="F10" s="14">
+        <f>SUM('Week 6:Week 27'!H13)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
+        <f>F10/(B1/100)</f>
+        <v>0</v>
+      </c>
       <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5">
+        <f>SUM('Week 6:Week 27'!J8,F11)</f>
+        <v>186</v>
+      </c>
+      <c r="C11" s="19">
+        <f>B11/(B1/100)</f>
+        <v>100</v>
+      </c>
+      <c r="D11" s="5">
+        <f>SUM('Week 6:Week 27'!H13)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="19">
+        <f>D11/(B1/100)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <f>SUM('Week 6:Week 27'!H14)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="18">
+        <f>F11/(B1/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2258,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2556,22 +2630,22 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="47.88671875" customWidth="1"/>
-    <col min="11" max="11" width="2.6640625" customWidth="1"/>
+    <col min="11" max="11" width="3.109375" customWidth="1"/>
+    <col min="12" max="12" width="47.88671875" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>12</v>
@@ -2594,27 +2668,41 @@
       <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="5">
+        <v>186</v>
+      </c>
+      <c r="J2" s="5">
+        <v>186</v>
+      </c>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2625,10 +2713,12 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2639,10 +2729,12 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2653,10 +2745,12 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2667,10 +2761,12 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2682,13 +2778,14 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5">
-        <f>SUM(B2+B3+B4+B5+B6)</f>
         <v>0</v>
       </c>
       <c r="C8" s="5">
@@ -2715,11 +2812,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" s="5">
+        <f>SUM(I2:I6)</f>
+        <v>186</v>
+      </c>
+      <c r="J8" s="5">
+        <f>SUM(J2:J6)</f>
+        <v>186</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2729,10 +2834,12 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2744,28 +2851,30 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" s="1"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="1"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2775,8 +2884,10 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2787,7 +2898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -5523,7 +5634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>